<commit_message>
docs(update): update data to 1.3 version
</commit_message>
<xml_diff>
--- a/开局.xlsx
+++ b/开局.xlsx
@@ -795,7 +795,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -812,9 +812,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1130,8 +1127,8 @@
   <sheetPr/>
   <dimension ref="A1:X30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="U33" sqref="U33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1222,12 +1219,12 @@
         <v>23</v>
       </c>
       <c r="B2">
-        <f>SUM(4500,X2,400)</f>
-        <v>4900</v>
+        <f>SUM(4500,X2,500)</f>
+        <v>5000</v>
       </c>
       <c r="C2">
-        <f>SUM(500,X2,4500)</f>
-        <v>5000</v>
+        <f>SUM(600,X2,4500)</f>
+        <v>5100</v>
       </c>
       <c r="D2">
         <f>SUM(-400,X2,4500)</f>
@@ -1294,16 +1291,16 @@
         <v>4800</v>
       </c>
       <c r="T2">
-        <f>SUM(4500,-400,X2)</f>
-        <v>4100</v>
+        <f>SUM(4500,-200,X2)</f>
+        <v>4300</v>
       </c>
       <c r="U2">
-        <f>SUM(4500,200,X2)</f>
-        <v>4700</v>
+        <f>SUM(4500,400,X2)</f>
+        <v>4900</v>
       </c>
       <c r="V2">
-        <f>SUM(4500,-500,X2)</f>
-        <v>4000</v>
+        <f>SUM(4500,-300,X2)</f>
+        <v>4200</v>
       </c>
       <c r="X2" s="2">
         <v>0</v>
@@ -1314,91 +1311,91 @@
         <v>24</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B18" si="0">SUM(4500,X3,400)</f>
-        <v>5100</v>
+        <f t="shared" ref="B3:B18" si="0">SUM(4500,X3,500)</f>
+        <v>5400</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C18" si="1">SUM(500,X3,4500)</f>
-        <v>5200</v>
+        <f t="shared" ref="C3:C18" si="1">SUM(600,X3,4500)</f>
+        <v>5500</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D18" si="2">SUM(-400,X3,4500)</f>
-        <v>4300</v>
+        <v>4500</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E18" si="3">SUM(4500,X3,0)</f>
-        <v>4700</v>
+        <v>4900</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F18" si="4">SUM(4500,100,X3)</f>
-        <v>4800</v>
+        <v>5000</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G18" si="5">SUM(4500,200,X3)</f>
-        <v>4900</v>
+        <v>5100</v>
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H18" si="6">SUM(4500,-200,X3)</f>
-        <v>4500</v>
+        <v>4700</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I18" si="7">SUM(4500,-500,X3)</f>
-        <v>4200</v>
+        <v>4400</v>
       </c>
       <c r="J3">
         <f t="shared" ref="J3:J18" si="8">SUM(4500,-200,X3)</f>
-        <v>4500</v>
+        <v>4700</v>
       </c>
       <c r="K3">
         <f t="shared" ref="K3:K18" si="9">SUM(4500,200,X3)</f>
-        <v>4900</v>
+        <v>5100</v>
       </c>
       <c r="L3">
         <f t="shared" ref="L3:L18" si="10">SUM(4500,-500,X3)</f>
-        <v>4200</v>
+        <v>4400</v>
       </c>
       <c r="M3">
         <f t="shared" ref="M3:M18" si="11">SUM(4500,0,X3)</f>
-        <v>4700</v>
+        <v>4900</v>
       </c>
       <c r="N3">
         <f t="shared" ref="N3:N18" si="12">SUM(4500,700,X3)</f>
-        <v>5400</v>
+        <v>5600</v>
       </c>
       <c r="O3">
         <f t="shared" ref="O3:O18" si="13">SUM(4500,0,X3)</f>
-        <v>4700</v>
+        <v>4900</v>
       </c>
       <c r="P3">
         <f t="shared" ref="P3:P18" si="14">SUM(4500,100,X3)</f>
-        <v>4800</v>
+        <v>5000</v>
       </c>
       <c r="Q3">
         <f t="shared" ref="Q3:Q18" si="15">SUM(4500,-300,X3)</f>
-        <v>4400</v>
+        <v>4600</v>
       </c>
       <c r="R3">
         <f t="shared" ref="R3:R18" si="16">SUM(4500,200,X3)</f>
-        <v>4900</v>
+        <v>5100</v>
       </c>
       <c r="S3">
         <f t="shared" ref="S3:S18" si="17">SUM(4500,300,X3)</f>
-        <v>5000</v>
+        <v>5200</v>
       </c>
       <c r="T3">
-        <f t="shared" ref="T3:T18" si="18">SUM(4500,-400,X3)</f>
-        <v>4300</v>
+        <f t="shared" ref="T3:T18" si="18">SUM(4500,-200,X3)</f>
+        <v>4700</v>
       </c>
       <c r="U3">
-        <f t="shared" ref="U3:U18" si="19">SUM(4500,200,X3)</f>
-        <v>4900</v>
+        <f t="shared" ref="U3:U18" si="19">SUM(4500,400,X3)</f>
+        <v>5300</v>
       </c>
       <c r="V3">
-        <f t="shared" ref="V3:V18" si="20">SUM(4500,-500,X3)</f>
-        <v>4200</v>
+        <f t="shared" ref="V3:V18" si="20">SUM(4500,-300,X3)</f>
+        <v>4600</v>
       </c>
       <c r="X3" s="2">
-        <v>200</v>
+        <v>400</v>
       </c>
     </row>
     <row r="4" spans="1:24">
@@ -1407,11 +1404,11 @@
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
-        <v>5000</v>
+        <v>5100</v>
       </c>
       <c r="C4">
         <f t="shared" si="1"/>
-        <v>5100</v>
+        <v>5200</v>
       </c>
       <c r="D4">
         <f t="shared" si="2"/>
@@ -1479,15 +1476,15 @@
       </c>
       <c r="T4">
         <f t="shared" si="18"/>
-        <v>4200</v>
+        <v>4400</v>
       </c>
       <c r="U4">
         <f t="shared" si="19"/>
-        <v>4800</v>
+        <v>5000</v>
       </c>
       <c r="V4">
         <f t="shared" si="20"/>
-        <v>4100</v>
+        <v>4300</v>
       </c>
       <c r="X4" s="2">
         <v>100</v>
@@ -1499,11 +1496,11 @@
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>4700</v>
+        <v>4800</v>
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
-        <v>4800</v>
+        <v>4900</v>
       </c>
       <c r="D5">
         <f t="shared" si="2"/>
@@ -1571,15 +1568,15 @@
       </c>
       <c r="T5">
         <f t="shared" si="18"/>
-        <v>3900</v>
+        <v>4100</v>
       </c>
       <c r="U5">
         <f t="shared" si="19"/>
-        <v>4500</v>
+        <v>4700</v>
       </c>
       <c r="V5">
         <f t="shared" si="20"/>
-        <v>3800</v>
+        <v>4000</v>
       </c>
       <c r="X5" s="2">
         <v>-200</v>
@@ -1591,11 +1588,11 @@
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>5400</v>
+        <v>5500</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>5500</v>
+        <v>5600</v>
       </c>
       <c r="D6">
         <f t="shared" si="2"/>
@@ -1638,7 +1635,7 @@
         <v>5000</v>
       </c>
       <c r="N6" s="3">
-        <f>SUM(4500,700,X6)</f>
+        <f t="shared" si="12"/>
         <v>5700</v>
       </c>
       <c r="O6">
@@ -1663,15 +1660,15 @@
       </c>
       <c r="T6">
         <f t="shared" si="18"/>
-        <v>4600</v>
+        <v>4800</v>
       </c>
       <c r="U6">
         <f t="shared" si="19"/>
-        <v>5200</v>
+        <v>5400</v>
       </c>
       <c r="V6">
         <f t="shared" si="20"/>
-        <v>4500</v>
+        <v>4700</v>
       </c>
       <c r="X6" s="2">
         <v>500</v>
@@ -1683,75 +1680,75 @@
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>4900</v>
+        <v>4800</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>5000</v>
+        <v>4900</v>
       </c>
       <c r="D7">
         <f t="shared" si="2"/>
-        <v>4100</v>
+        <v>3900</v>
       </c>
       <c r="E7">
         <f t="shared" si="3"/>
-        <v>4500</v>
+        <v>4300</v>
       </c>
       <c r="F7">
         <f t="shared" si="4"/>
-        <v>4600</v>
+        <v>4400</v>
       </c>
       <c r="G7">
         <f t="shared" si="5"/>
-        <v>4700</v>
+        <v>4500</v>
       </c>
       <c r="H7">
         <f t="shared" si="6"/>
-        <v>4300</v>
+        <v>4100</v>
       </c>
       <c r="I7">
         <f t="shared" si="7"/>
-        <v>4000</v>
+        <v>3800</v>
       </c>
       <c r="J7">
         <f t="shared" si="8"/>
-        <v>4300</v>
+        <v>4100</v>
       </c>
       <c r="K7">
         <f t="shared" si="9"/>
-        <v>4700</v>
+        <v>4500</v>
       </c>
       <c r="L7">
         <f t="shared" si="10"/>
-        <v>4000</v>
+        <v>3800</v>
       </c>
       <c r="M7">
         <f t="shared" si="11"/>
-        <v>4500</v>
+        <v>4300</v>
       </c>
       <c r="N7">
         <f t="shared" si="12"/>
-        <v>5200</v>
+        <v>5000</v>
       </c>
       <c r="O7">
         <f t="shared" si="13"/>
-        <v>4500</v>
+        <v>4300</v>
       </c>
       <c r="P7">
         <f t="shared" si="14"/>
-        <v>4600</v>
+        <v>4400</v>
       </c>
       <c r="Q7">
         <f t="shared" si="15"/>
-        <v>4200</v>
+        <v>4000</v>
       </c>
       <c r="R7">
         <f t="shared" si="16"/>
-        <v>4700</v>
+        <v>4500</v>
       </c>
       <c r="S7">
         <f t="shared" si="17"/>
-        <v>4800</v>
+        <v>4600</v>
       </c>
       <c r="T7">
         <f t="shared" si="18"/>
@@ -1766,7 +1763,7 @@
         <v>4000</v>
       </c>
       <c r="X7" s="2">
-        <v>0</v>
+        <v>-200</v>
       </c>
     </row>
     <row r="8" spans="1:24">
@@ -1775,11 +1772,11 @@
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>5000</v>
+        <v>5100</v>
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>5100</v>
+        <v>5200</v>
       </c>
       <c r="D8">
         <f t="shared" si="2"/>
@@ -1847,15 +1844,15 @@
       </c>
       <c r="T8">
         <f t="shared" si="18"/>
-        <v>4200</v>
+        <v>4400</v>
       </c>
       <c r="U8">
         <f t="shared" si="19"/>
-        <v>4800</v>
+        <v>5000</v>
       </c>
       <c r="V8">
         <f t="shared" si="20"/>
-        <v>4100</v>
+        <v>4300</v>
       </c>
       <c r="X8" s="2">
         <v>100</v>
@@ -1867,11 +1864,11 @@
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>5100</v>
+        <v>5200</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
-        <v>5200</v>
+        <v>5300</v>
       </c>
       <c r="D9">
         <f t="shared" si="2"/>
@@ -1939,15 +1936,15 @@
       </c>
       <c r="T9">
         <f t="shared" si="18"/>
-        <v>4300</v>
+        <v>4500</v>
       </c>
       <c r="U9">
         <f t="shared" si="19"/>
-        <v>4900</v>
+        <v>5100</v>
       </c>
       <c r="V9">
         <f t="shared" si="20"/>
-        <v>4200</v>
+        <v>4400</v>
       </c>
       <c r="X9" s="2">
         <v>200</v>
@@ -1959,11 +1956,11 @@
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>4900</v>
+        <v>5000</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
-        <v>5000</v>
+        <v>5100</v>
       </c>
       <c r="D10">
         <f t="shared" si="2"/>
@@ -2031,15 +2028,15 @@
       </c>
       <c r="T10">
         <f t="shared" si="18"/>
-        <v>4100</v>
+        <v>4300</v>
       </c>
       <c r="U10">
         <f t="shared" si="19"/>
-        <v>4700</v>
+        <v>4900</v>
       </c>
       <c r="V10">
         <f t="shared" si="20"/>
-        <v>4000</v>
+        <v>4200</v>
       </c>
       <c r="X10" s="2">
         <v>0</v>
@@ -2051,11 +2048,11 @@
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
-        <v>4900</v>
+        <v>5000</v>
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
-        <v>5000</v>
+        <v>5100</v>
       </c>
       <c r="D11">
         <f t="shared" si="2"/>
@@ -2123,15 +2120,15 @@
       </c>
       <c r="T11">
         <f t="shared" si="18"/>
-        <v>4100</v>
+        <v>4300</v>
       </c>
       <c r="U11">
         <f t="shared" si="19"/>
-        <v>4700</v>
+        <v>4900</v>
       </c>
       <c r="V11">
         <f t="shared" si="20"/>
-        <v>4000</v>
+        <v>4200</v>
       </c>
       <c r="X11" s="2">
         <v>0</v>
@@ -2143,11 +2140,11 @@
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
-        <v>4600</v>
+        <v>4700</v>
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
-        <v>4700</v>
+        <v>4800</v>
       </c>
       <c r="D12">
         <f t="shared" si="2"/>
@@ -2215,15 +2212,15 @@
       </c>
       <c r="T12">
         <f t="shared" si="18"/>
-        <v>3800</v>
+        <v>4000</v>
       </c>
       <c r="U12">
         <f t="shared" si="19"/>
-        <v>4400</v>
+        <v>4600</v>
       </c>
       <c r="V12">
         <f t="shared" si="20"/>
-        <v>3700</v>
+        <v>3900</v>
       </c>
       <c r="X12" s="2">
         <v>-300</v>
@@ -2235,11 +2232,11 @@
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
-        <v>5100</v>
+        <v>5200</v>
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
-        <v>5200</v>
+        <v>5300</v>
       </c>
       <c r="D13">
         <f t="shared" si="2"/>
@@ -2307,15 +2304,15 @@
       </c>
       <c r="T13">
         <f t="shared" si="18"/>
-        <v>4300</v>
+        <v>4500</v>
       </c>
       <c r="U13">
         <f t="shared" si="19"/>
-        <v>4900</v>
+        <v>5100</v>
       </c>
       <c r="V13">
         <f t="shared" si="20"/>
-        <v>4200</v>
+        <v>4400</v>
       </c>
       <c r="X13" s="2">
         <v>200</v>
@@ -2327,11 +2324,11 @@
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
-        <v>5300</v>
+        <v>5400</v>
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
-        <v>5400</v>
+        <v>5500</v>
       </c>
       <c r="D14">
         <f t="shared" si="2"/>
@@ -2399,15 +2396,15 @@
       </c>
       <c r="T14">
         <f t="shared" si="18"/>
-        <v>4500</v>
+        <v>4700</v>
       </c>
       <c r="U14">
         <f t="shared" si="19"/>
-        <v>5100</v>
+        <v>5300</v>
       </c>
       <c r="V14">
         <f t="shared" si="20"/>
-        <v>4400</v>
+        <v>4600</v>
       </c>
       <c r="X14" s="2">
         <v>400</v>
@@ -2419,11 +2416,11 @@
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
-        <v>5200</v>
+        <v>5300</v>
       </c>
       <c r="C15">
         <f t="shared" si="1"/>
-        <v>5300</v>
+        <v>5400</v>
       </c>
       <c r="D15">
         <f t="shared" si="2"/>
@@ -2491,15 +2488,15 @@
       </c>
       <c r="T15">
         <f t="shared" si="18"/>
-        <v>4400</v>
+        <v>4600</v>
       </c>
       <c r="U15">
         <f t="shared" si="19"/>
-        <v>5000</v>
+        <v>5200</v>
       </c>
       <c r="V15">
         <f t="shared" si="20"/>
-        <v>4300</v>
+        <v>4500</v>
       </c>
       <c r="X15" s="2">
         <v>300</v>
@@ -2511,11 +2508,11 @@
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
-        <v>4700</v>
+        <v>4800</v>
       </c>
       <c r="C16">
         <f t="shared" si="1"/>
-        <v>4800</v>
+        <v>4900</v>
       </c>
       <c r="D16">
         <f t="shared" si="2"/>
@@ -2583,15 +2580,15 @@
       </c>
       <c r="T16">
         <f t="shared" si="18"/>
-        <v>3900</v>
+        <v>4100</v>
       </c>
       <c r="U16">
         <f t="shared" si="19"/>
-        <v>4500</v>
+        <v>4700</v>
       </c>
       <c r="V16">
         <f t="shared" si="20"/>
-        <v>3800</v>
+        <v>4000</v>
       </c>
       <c r="X16" s="2">
         <v>-200</v>
@@ -2603,11 +2600,11 @@
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
-        <v>4900</v>
+        <v>5000</v>
       </c>
       <c r="C17">
         <f t="shared" si="1"/>
-        <v>5000</v>
+        <v>5100</v>
       </c>
       <c r="D17">
         <f t="shared" si="2"/>
@@ -2675,15 +2672,15 @@
       </c>
       <c r="T17">
         <f t="shared" si="18"/>
-        <v>4100</v>
+        <v>4300</v>
       </c>
       <c r="U17">
         <f t="shared" si="19"/>
-        <v>4700</v>
+        <v>4900</v>
       </c>
       <c r="V17">
         <f t="shared" si="20"/>
-        <v>4000</v>
+        <v>4200</v>
       </c>
       <c r="X17" s="2">
         <v>0</v>
@@ -2703,95 +2700,95 @@
       </c>
       <c r="D18">
         <f t="shared" si="2"/>
-        <v>3700</v>
+        <v>3600</v>
       </c>
       <c r="E18">
         <f t="shared" si="3"/>
-        <v>4100</v>
+        <v>4000</v>
       </c>
       <c r="F18">
         <f t="shared" si="4"/>
-        <v>4200</v>
+        <v>4100</v>
       </c>
       <c r="G18">
         <f t="shared" si="5"/>
-        <v>4300</v>
+        <v>4200</v>
       </c>
       <c r="H18">
         <f t="shared" si="6"/>
-        <v>3900</v>
+        <v>3800</v>
       </c>
       <c r="I18" s="4">
         <f t="shared" si="7"/>
-        <v>3600</v>
+        <v>3500</v>
       </c>
       <c r="J18">
         <f t="shared" si="8"/>
-        <v>3900</v>
+        <v>3800</v>
       </c>
       <c r="K18">
         <f t="shared" si="9"/>
-        <v>4300</v>
+        <v>4200</v>
       </c>
       <c r="L18" s="4">
         <f t="shared" si="10"/>
-        <v>3600</v>
+        <v>3500</v>
       </c>
       <c r="M18">
         <f t="shared" si="11"/>
-        <v>4100</v>
+        <v>4000</v>
       </c>
       <c r="N18">
         <f t="shared" si="12"/>
-        <v>4800</v>
+        <v>4700</v>
       </c>
       <c r="O18">
         <f t="shared" si="13"/>
-        <v>4100</v>
+        <v>4000</v>
       </c>
       <c r="P18">
         <f t="shared" si="14"/>
-        <v>4200</v>
+        <v>4100</v>
       </c>
       <c r="Q18">
         <f t="shared" si="15"/>
-        <v>3800</v>
+        <v>3700</v>
       </c>
       <c r="R18">
         <f t="shared" si="16"/>
-        <v>4300</v>
+        <v>4200</v>
       </c>
       <c r="S18">
         <f t="shared" si="17"/>
-        <v>4400</v>
+        <v>4300</v>
       </c>
       <c r="T18">
         <f t="shared" si="18"/>
-        <v>3700</v>
+        <v>3800</v>
       </c>
       <c r="U18">
         <f t="shared" si="19"/>
-        <v>4300</v>
-      </c>
-      <c r="V18" s="4">
+        <v>4400</v>
+      </c>
+      <c r="V18">
         <f t="shared" si="20"/>
-        <v>3600</v>
+        <v>3700</v>
       </c>
       <c r="X18" s="2">
-        <v>-400</v>
+        <v>-500</v>
       </c>
     </row>
     <row r="19" spans="1:24">
       <c r="A19" t="s">
         <v>21</v>
       </c>
-      <c r="W19" s="6">
+      <c r="W19" s="1">
         <f>SUM(A1,W20,X19)</f>
-        <v>4548.17927170868</v>
+        <v>4580.39215686274</v>
       </c>
       <c r="X19" s="5">
         <f>AVERAGE(X2:X18)</f>
-        <v>52.9411764705882</v>
+        <v>47.0588235294118</v>
       </c>
     </row>
     <row r="20" spans="1:23">
@@ -2799,10 +2796,10 @@
         <v>22</v>
       </c>
       <c r="B20" s="2">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="C20" s="2">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="D20" s="2">
         <v>-400</v>
@@ -2853,17 +2850,17 @@
         <v>300</v>
       </c>
       <c r="T20" s="2">
-        <v>-400</v>
+        <v>-200</v>
       </c>
       <c r="U20" s="2">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="V20" s="2">
-        <v>-500</v>
+        <v>-300</v>
       </c>
       <c r="W20">
         <f>AVERAGE(B20:V20)</f>
-        <v>-4.76190476190476</v>
+        <v>33.3333333333333</v>
       </c>
     </row>
     <row r="30" spans="15:15">

</xml_diff>